<commit_message>
Ajout les paramètres headless browsers
</commit_message>
<xml_diff>
--- a/ExcelData.xlsx
+++ b/ExcelData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1181" uniqueCount="280">
   <si>
     <t>ID</t>
   </si>
@@ -795,6 +795,75 @@
   </si>
   <si>
     <t>En plein discours, le Président des États-Unis est victime d'une tentative d'assassinat</t>
+  </si>
+  <si>
+    <t>10-oct.-22</t>
+  </si>
+  <si>
+    <t>Forains, gens du voyage : révélations sur une économie secrète</t>
+  </si>
+  <si>
+    <t>Parmi les mystères qui les entourent, le plus opaque est celui de l’argent</t>
+  </si>
+  <si>
+    <t>Gypsies et travellers</t>
+  </si>
+  <si>
+    <t>Qui sont ces gitans anglais qui fascinent et dérangent à la fois ?</t>
+  </si>
+  <si>
+    <t>Inspirée d'Au bonheur des dames, d'Émile Zola</t>
+  </si>
+  <si>
+    <t>À la fin du XIXe siècle, le premier grand magasin du nord de l'Angleterre ouvre ses portes</t>
+  </si>
+  <si>
+    <t>11-oct.-22</t>
+  </si>
+  <si>
+    <t>Pluie d'amour, dispute et choix décisif</t>
+  </si>
+  <si>
+    <t>Les séjours chez les agriculteurs se suivent mais ne se ressemblent pas</t>
+  </si>
+  <si>
+    <t>Le contrat</t>
+  </si>
+  <si>
+    <t>Melanight décide de s'allier avec Maeva</t>
+  </si>
+  <si>
+    <t>Les secrets d'une construction réussie</t>
+  </si>
+  <si>
+    <t>Bien s'entourer, une étape clé de votre projet</t>
+  </si>
+  <si>
+    <t>17-oct.-22</t>
+  </si>
+  <si>
+    <t>Le nouveau scandale des enfants placés</t>
+  </si>
+  <si>
+    <t>Des familles d'accueil aux hôtels sociaux, enquête sur les défaillances d'un système</t>
+  </si>
+  <si>
+    <t>Mozambique : le paradis sous la menace</t>
+  </si>
+  <si>
+    <t>Entre richesses naturelles et conflit armé, enquête au cœur d'un pays au rêve brisé</t>
+  </si>
+  <si>
+    <t>Une expérience inédite</t>
+  </si>
+  <si>
+    <t>Revivez ce live exceptionnel avec Cyril Lignac</t>
+  </si>
+  <si>
+    <t>Keira Knightley et Sienna Miller au sommet de leur art</t>
+  </si>
+  <si>
+    <t>Une chanteuse de cabaret recroise son premier amour, devenu poète et marié</t>
   </si>
 </sst>
 </file>
@@ -1215,7 +1284,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C338"/>
+  <dimension ref="A1:C436"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
       <selection activeCell="E66" sqref="E66"/>
@@ -4470,6 +4539,970 @@
       </c>
       <c r="C338" t="s">
         <v>256</v>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="s">
+        <v>28</v>
+      </c>
+      <c r="B340" t="s">
+        <v>258</v>
+      </c>
+      <c r="C340" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="s">
+        <v>31</v>
+      </c>
+      <c r="B341" t="s">
+        <v>249</v>
+      </c>
+      <c r="C341" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="s">
+        <v>34</v>
+      </c>
+      <c r="B342" t="s">
+        <v>260</v>
+      </c>
+      <c r="C342" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="s">
+        <v>42</v>
+      </c>
+      <c r="B343" t="s">
+        <v>262</v>
+      </c>
+      <c r="C343" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="s">
+        <v>28</v>
+      </c>
+      <c r="B345" t="s">
+        <v>265</v>
+      </c>
+      <c r="C345" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="s">
+        <v>31</v>
+      </c>
+      <c r="B346" t="s">
+        <v>249</v>
+      </c>
+      <c r="C346" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="s">
+        <v>34</v>
+      </c>
+      <c r="B347" t="s">
+        <v>267</v>
+      </c>
+      <c r="C347" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="s">
+        <v>42</v>
+      </c>
+      <c r="B348" t="s">
+        <v>269</v>
+      </c>
+      <c r="C348" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="s">
+        <v>58</v>
+      </c>
+      <c r="B349" t="s">
+        <v>262</v>
+      </c>
+      <c r="C349" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="s">
+        <v>28</v>
+      </c>
+      <c r="B351" t="s">
+        <v>265</v>
+      </c>
+      <c r="C351" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="s">
+        <v>31</v>
+      </c>
+      <c r="B352" t="s">
+        <v>249</v>
+      </c>
+      <c r="C352" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="s">
+        <v>34</v>
+      </c>
+      <c r="B353" t="s">
+        <v>267</v>
+      </c>
+      <c r="C353" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="s">
+        <v>42</v>
+      </c>
+      <c r="B354" t="s">
+        <v>269</v>
+      </c>
+      <c r="C354" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="s">
+        <v>58</v>
+      </c>
+      <c r="B355" t="s">
+        <v>262</v>
+      </c>
+      <c r="C355" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="s">
+        <v>28</v>
+      </c>
+      <c r="B357" t="s">
+        <v>272</v>
+      </c>
+      <c r="C357" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="s">
+        <v>31</v>
+      </c>
+      <c r="B358" t="s">
+        <v>249</v>
+      </c>
+      <c r="C358" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="s">
+        <v>34</v>
+      </c>
+      <c r="B359" t="s">
+        <v>274</v>
+      </c>
+      <c r="C359" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="s">
+        <v>42</v>
+      </c>
+      <c r="B360" t="s">
+        <v>276</v>
+      </c>
+      <c r="C360" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="s">
+        <v>58</v>
+      </c>
+      <c r="B361" t="s">
+        <v>278</v>
+      </c>
+      <c r="C361" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="s">
+        <v>28</v>
+      </c>
+      <c r="B363" t="s">
+        <v>272</v>
+      </c>
+      <c r="C363" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="s">
+        <v>31</v>
+      </c>
+      <c r="B364" t="s">
+        <v>249</v>
+      </c>
+      <c r="C364" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="s">
+        <v>34</v>
+      </c>
+      <c r="B365" t="s">
+        <v>274</v>
+      </c>
+      <c r="C365" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="s">
+        <v>42</v>
+      </c>
+      <c r="B366" t="s">
+        <v>276</v>
+      </c>
+      <c r="C366" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="s">
+        <v>58</v>
+      </c>
+      <c r="B367" t="s">
+        <v>278</v>
+      </c>
+      <c r="C367" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="s">
+        <v>28</v>
+      </c>
+      <c r="B369" t="s">
+        <v>272</v>
+      </c>
+      <c r="C369" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="s">
+        <v>31</v>
+      </c>
+      <c r="B370" t="s">
+        <v>249</v>
+      </c>
+      <c r="C370" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="s">
+        <v>34</v>
+      </c>
+      <c r="B371" t="s">
+        <v>274</v>
+      </c>
+      <c r="C371" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="s">
+        <v>42</v>
+      </c>
+      <c r="B372" t="s">
+        <v>276</v>
+      </c>
+      <c r="C372" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="s">
+        <v>58</v>
+      </c>
+      <c r="B373" t="s">
+        <v>278</v>
+      </c>
+      <c r="C373" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="s">
+        <v>28</v>
+      </c>
+      <c r="B375" t="s">
+        <v>272</v>
+      </c>
+      <c r="C375" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="s">
+        <v>31</v>
+      </c>
+      <c r="B376" t="s">
+        <v>249</v>
+      </c>
+      <c r="C376" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="s">
+        <v>34</v>
+      </c>
+      <c r="B377" t="s">
+        <v>274</v>
+      </c>
+      <c r="C377" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="s">
+        <v>42</v>
+      </c>
+      <c r="B378" t="s">
+        <v>276</v>
+      </c>
+      <c r="C378" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="s">
+        <v>58</v>
+      </c>
+      <c r="B379" t="s">
+        <v>278</v>
+      </c>
+      <c r="C379" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="s">
+        <v>28</v>
+      </c>
+      <c r="B381" t="s">
+        <v>272</v>
+      </c>
+      <c r="C381" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="s">
+        <v>31</v>
+      </c>
+      <c r="B382" t="s">
+        <v>187</v>
+      </c>
+      <c r="C382" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="s">
+        <v>34</v>
+      </c>
+      <c r="B383" t="s">
+        <v>187</v>
+      </c>
+      <c r="C383" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="s">
+        <v>42</v>
+      </c>
+      <c r="B384" t="s">
+        <v>187</v>
+      </c>
+      <c r="C384" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="s">
+        <v>58</v>
+      </c>
+      <c r="B385" t="s">
+        <v>187</v>
+      </c>
+      <c r="C385" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="s">
+        <v>28</v>
+      </c>
+      <c r="B387" t="s">
+        <v>272</v>
+      </c>
+      <c r="C387" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="s">
+        <v>31</v>
+      </c>
+      <c r="B388" t="s">
+        <v>187</v>
+      </c>
+      <c r="C388" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="s">
+        <v>34</v>
+      </c>
+      <c r="B389" t="s">
+        <v>187</v>
+      </c>
+      <c r="C389" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="s">
+        <v>42</v>
+      </c>
+      <c r="B390" t="s">
+        <v>187</v>
+      </c>
+      <c r="C390" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="s">
+        <v>58</v>
+      </c>
+      <c r="B391" t="s">
+        <v>187</v>
+      </c>
+      <c r="C391" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="s">
+        <v>28</v>
+      </c>
+      <c r="B393" t="s">
+        <v>272</v>
+      </c>
+      <c r="C393" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="s">
+        <v>31</v>
+      </c>
+      <c r="B394" t="s">
+        <v>187</v>
+      </c>
+      <c r="C394" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="s">
+        <v>34</v>
+      </c>
+      <c r="B395" t="s">
+        <v>187</v>
+      </c>
+      <c r="C395" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="s">
+        <v>42</v>
+      </c>
+      <c r="B396" t="s">
+        <v>187</v>
+      </c>
+      <c r="C396" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="s">
+        <v>58</v>
+      </c>
+      <c r="B397" t="s">
+        <v>187</v>
+      </c>
+      <c r="C397" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="s">
+        <v>28</v>
+      </c>
+      <c r="B399" t="s">
+        <v>272</v>
+      </c>
+      <c r="C399" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="s">
+        <v>31</v>
+      </c>
+      <c r="B400" t="s">
+        <v>187</v>
+      </c>
+      <c r="C400" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="s">
+        <v>34</v>
+      </c>
+      <c r="B401" t="s">
+        <v>274</v>
+      </c>
+      <c r="C401" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="s">
+        <v>42</v>
+      </c>
+      <c r="B402" t="s">
+        <v>276</v>
+      </c>
+      <c r="C402" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="s">
+        <v>58</v>
+      </c>
+      <c r="B403" t="s">
+        <v>278</v>
+      </c>
+      <c r="C403" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="s">
+        <v>28</v>
+      </c>
+      <c r="B405" t="s">
+        <v>272</v>
+      </c>
+      <c r="C405" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="s">
+        <v>31</v>
+      </c>
+      <c r="B406" t="s">
+        <v>249</v>
+      </c>
+      <c r="C406" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="s">
+        <v>34</v>
+      </c>
+      <c r="B407" t="s">
+        <v>274</v>
+      </c>
+      <c r="C407" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="s">
+        <v>42</v>
+      </c>
+      <c r="B408" t="s">
+        <v>276</v>
+      </c>
+      <c r="C408" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="s">
+        <v>58</v>
+      </c>
+      <c r="B409" t="s">
+        <v>278</v>
+      </c>
+      <c r="C409" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="s">
+        <v>28</v>
+      </c>
+      <c r="B411" t="s">
+        <v>272</v>
+      </c>
+      <c r="C411" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="s">
+        <v>31</v>
+      </c>
+      <c r="B412" t="s">
+        <v>249</v>
+      </c>
+      <c r="C412" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="s">
+        <v>34</v>
+      </c>
+      <c r="B413" t="s">
+        <v>274</v>
+      </c>
+      <c r="C413" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="s">
+        <v>42</v>
+      </c>
+      <c r="B414" t="s">
+        <v>276</v>
+      </c>
+      <c r="C414" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="s">
+        <v>58</v>
+      </c>
+      <c r="B415" t="s">
+        <v>278</v>
+      </c>
+      <c r="C415" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="s">
+        <v>28</v>
+      </c>
+      <c r="B417" t="s">
+        <v>272</v>
+      </c>
+      <c r="C417" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="s">
+        <v>31</v>
+      </c>
+      <c r="B418" t="s">
+        <v>249</v>
+      </c>
+      <c r="C418" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="s">
+        <v>34</v>
+      </c>
+      <c r="B419" t="s">
+        <v>274</v>
+      </c>
+      <c r="C419" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="s">
+        <v>42</v>
+      </c>
+      <c r="B420" t="s">
+        <v>276</v>
+      </c>
+      <c r="C420" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="s">
+        <v>58</v>
+      </c>
+      <c r="B421" t="s">
+        <v>278</v>
+      </c>
+      <c r="C421" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="s">
+        <v>28</v>
+      </c>
+      <c r="B425" t="s">
+        <v>272</v>
+      </c>
+      <c r="C425" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="s">
+        <v>31</v>
+      </c>
+      <c r="B426" t="s">
+        <v>249</v>
+      </c>
+      <c r="C426" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="s">
+        <v>34</v>
+      </c>
+      <c r="B427" t="s">
+        <v>274</v>
+      </c>
+      <c r="C427" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="s">
+        <v>42</v>
+      </c>
+      <c r="B428" t="s">
+        <v>276</v>
+      </c>
+      <c r="C428" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="s">
+        <v>58</v>
+      </c>
+      <c r="B429" t="s">
+        <v>278</v>
+      </c>
+      <c r="C429" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="s">
+        <v>28</v>
+      </c>
+      <c r="B432" t="s">
+        <v>272</v>
+      </c>
+      <c r="C432" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="s">
+        <v>31</v>
+      </c>
+      <c r="B433" t="s">
+        <v>249</v>
+      </c>
+      <c r="C433" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="s">
+        <v>34</v>
+      </c>
+      <c r="B434" t="s">
+        <v>274</v>
+      </c>
+      <c r="C434" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="s">
+        <v>42</v>
+      </c>
+      <c r="B435" t="s">
+        <v>276</v>
+      </c>
+      <c r="C435" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="s">
+        <v>58</v>
+      </c>
+      <c r="B436" t="s">
+        <v>278</v>
+      </c>
+      <c r="C436" t="s">
+        <v>279</v>
       </c>
     </row>
   </sheetData>

</xml_diff>